<commit_message>
Update 1조 PerfectSolution 통합테스트 시나리오 - 민기.xlsx
</commit_message>
<xml_diff>
--- a/6. 1조 테스트시나리오/1조 PerfectSolution 통합테스트 시나리오 - 민기.xlsx
+++ b/6. 1조 테스트시나리오/1조 PerfectSolution 통합테스트 시나리오 - 민기.xlsx
@@ -53499,114 +53499,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>조치대기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>중인</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>항목에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>따른</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>조치코드</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>미출력</t>
-    </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>정상동작</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -53695,6 +53587,143 @@
   </si>
   <si>
     <t>Ｘ</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조치대기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>항목에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>따른</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조치코드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">미출력
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-&gt; url </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>문제</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(localhost)</t>
+    </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -54770,7 +54799,7 @@
   </sheetPr>
   <dimension ref="A1:N226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E70" workbookViewId="0">
       <selection activeCell="M100" sqref="M100"/>
     </sheetView>
   </sheetViews>
@@ -56489,7 +56518,7 @@
       <c r="H84" s="16"/>
       <c r="I84" s="16"/>
       <c r="J84" s="50" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K84" s="118" t="s">
         <v>508</v>
@@ -56512,7 +56541,7 @@
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
       <c r="J85" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K85" s="48" t="s">
         <v>512</v>
@@ -56535,7 +56564,7 @@
       <c r="H86" s="16"/>
       <c r="I86" s="16"/>
       <c r="J86" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K86" s="47" t="s">
         <v>513</v>
@@ -56558,7 +56587,7 @@
       <c r="H87" s="16"/>
       <c r="I87" s="16"/>
       <c r="J87" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K87" s="47" t="s">
         <v>514</v>
@@ -56581,7 +56610,7 @@
       <c r="H88" s="16"/>
       <c r="I88" s="16"/>
       <c r="J88" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K88" s="47" t="s">
         <v>506</v>
@@ -56604,7 +56633,7 @@
       <c r="H89" s="16"/>
       <c r="I89" s="16"/>
       <c r="J89" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K89" s="47" t="s">
         <v>507</v>
@@ -56627,7 +56656,7 @@
       <c r="H90" s="16"/>
       <c r="I90" s="16"/>
       <c r="J90" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K90" s="47" t="s">
         <v>509</v>
@@ -56650,7 +56679,7 @@
       <c r="H91" s="16"/>
       <c r="I91" s="16"/>
       <c r="J91" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K91" s="47" t="s">
         <v>510</v>
@@ -56677,7 +56706,7 @@
       <c r="H92" s="16"/>
       <c r="I92" s="16"/>
       <c r="J92" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K92" s="47" t="s">
         <v>508</v>
@@ -56700,7 +56729,7 @@
       <c r="H93" s="16"/>
       <c r="I93" s="16"/>
       <c r="J93" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K93" s="47" t="s">
         <v>511</v>
@@ -56723,7 +56752,7 @@
       <c r="H94" s="16"/>
       <c r="I94" s="16"/>
       <c r="J94" s="50" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K94" s="41" t="s">
         <v>516</v>
@@ -56746,7 +56775,7 @@
       <c r="H95" s="16"/>
       <c r="I95" s="16"/>
       <c r="J95" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K95" s="47" t="s">
         <v>515</v>
@@ -56769,7 +56798,7 @@
       <c r="H96" s="16"/>
       <c r="I96" s="16"/>
       <c r="J96" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K96" s="47" t="s">
         <v>517</v>
@@ -56798,7 +56827,7 @@
       <c r="H97" s="16"/>
       <c r="I97" s="16"/>
       <c r="J97" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K97" s="118" t="s">
         <v>509</v>
@@ -56821,7 +56850,7 @@
       <c r="H98" s="16"/>
       <c r="I98" s="16"/>
       <c r="J98" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K98" s="118" t="s">
         <v>508</v>
@@ -56844,7 +56873,7 @@
       <c r="H99" s="16"/>
       <c r="I99" s="16"/>
       <c r="J99" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K99" s="118" t="s">
         <v>509</v>
@@ -56867,10 +56896,10 @@
       <c r="H100" s="16"/>
       <c r="I100" s="16"/>
       <c r="J100" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K100" s="118" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L100" s="16"/>
       <c r="M100" s="29"/>
@@ -56890,7 +56919,7 @@
       <c r="H101" s="16"/>
       <c r="I101" s="16"/>
       <c r="J101" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K101" s="119" t="s">
         <v>509</v>
@@ -56898,7 +56927,7 @@
       <c r="L101" s="16"/>
       <c r="M101" s="29"/>
     </row>
-    <row r="102" spans="1:13" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A102" s="56"/>
       <c r="B102" s="56"/>
       <c r="C102" s="56"/>
@@ -56913,10 +56942,10 @@
       <c r="H102" s="16"/>
       <c r="I102" s="16"/>
       <c r="J102" s="50" t="s">
+        <v>525</v>
+      </c>
+      <c r="K102" s="48" t="s">
         <v>526</v>
-      </c>
-      <c r="K102" s="48" t="s">
-        <v>519</v>
       </c>
       <c r="L102" s="16"/>
       <c r="M102" s="29"/>
@@ -56936,10 +56965,10 @@
       <c r="H103" s="16"/>
       <c r="I103" s="16"/>
       <c r="J103" s="50" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K103" s="48" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L103" s="16"/>
       <c r="M103" s="29"/>

</xml_diff>